<commit_message>
Fix: Stop tracking .venv folder
</commit_message>
<xml_diff>
--- a/data/books6.xlsx
+++ b/data/books6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web_dev\next.js\ML_project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Node\ReadSphere\ReadSphere_ML_Service\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413E15B6-3201-4444-A323-3563D7C48DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164FF1BA-0170-4945-AD80-E2883CEAD869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5090A77F-BB31-4DCF-A932-A06C12D3F666}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5090A77F-BB31-4DCF-A932-A06C12D3F666}"/>
   </bookViews>
   <sheets>
     <sheet name="Books2" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="381">
   <si>
-    <t>BOOK_ID</t>
-  </si>
-  <si>
     <t>BOOK_TITLE</t>
   </si>
   <si>
-    <t>BOOK_AURTHOR</t>
-  </si>
-  <si>
     <t>YEAR_P</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>LINK</t>
   </si>
   <si>
-    <t>GENERE</t>
-  </si>
-  <si>
     <t>LANGUAGE</t>
   </si>
   <si>
@@ -1177,6 +1168,15 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dgwsfoozs/image/upload/v1743402410/Screenshot_2025-03-31_114727_i2lwex.png</t>
+  </si>
+  <si>
+    <t>BOOK_AUTHOR</t>
+  </si>
+  <si>
+    <t>GENRE</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -1734,16 +1734,16 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{69105F29-BEE3-4535-AD9C-8BAD3EF02204}" name="Table1" displayName="Table1" ref="A1:K84" totalsRowShown="0">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8FF5A096-D28D-4B2F-B8CB-BB8966DD495D}" name="BOOK_ID"/>
+    <tableColumn id="1" xr3:uid="{8FF5A096-D28D-4B2F-B8CB-BB8966DD495D}" name="id"/>
     <tableColumn id="2" xr3:uid="{F944747D-FC01-4B2A-BA19-DB035F9D261A}" name="BOOK_TITLE"/>
-    <tableColumn id="3" xr3:uid="{824C6DE5-59F8-4F23-BC09-9A0ECF3EF5EF}" name="BOOK_AURTHOR"/>
+    <tableColumn id="3" xr3:uid="{824C6DE5-59F8-4F23-BC09-9A0ECF3EF5EF}" name="BOOK_AUTHOR"/>
     <tableColumn id="4" xr3:uid="{09C7D423-A738-4E49-ACE3-DB0573E0BAB7}" name="YEAR_P"/>
     <tableColumn id="5" xr3:uid="{A6D1F393-4A83-406C-B093-E05CF8C5D6B7}" name="PUBLISHER"/>
     <tableColumn id="6" xr3:uid="{2C4EC9F2-5E38-4ADE-8C29-6A8BE78F3393}" name="RATERS"/>
     <tableColumn id="7" xr3:uid="{AFCA0002-387A-4F25-A7D2-9FB80AC361C3}" name="A_RATINGS"/>
     <tableColumn id="8" xr3:uid="{53107771-4F36-4D46-9EAE-96272A62486E}" name="F_PAGE" dataCellStyle="Hyperlink"/>
     <tableColumn id="9" xr3:uid="{65F385E6-28DB-4DF3-9404-8DCD1B352F05}" name="LINK" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" xr3:uid="{2F9804FD-D2F3-4164-B530-BEB47C814C2B}" name="GENERE"/>
+    <tableColumn id="10" xr3:uid="{2F9804FD-D2F3-4164-B530-BEB47C814C2B}" name="GENRE"/>
     <tableColumn id="11" xr3:uid="{4EFE8015-B73F-4F36-A315-A30478EBFBD0}" name="LANGUAGE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2049,78 +2049,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6876ED-91AE-4ED4-BCCC-710AF588FC16}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="83" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="49.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="108.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="120.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" customWidth="1"/>
-    <col min="12" max="12" width="96.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="90.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.26953125" customWidth="1"/>
+    <col min="8" max="8" width="108.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="120.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="12" max="12" width="96.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="90.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>379</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>1650</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F2">
         <v>190</v>
@@ -2129,33 +2129,33 @@
         <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>2011</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>430</v>
@@ -2164,33 +2164,33 @@
         <v>7.6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>1997</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F4">
         <v>345</v>
@@ -2199,33 +2199,33 @@
         <v>6.3</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>1922</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F5">
         <v>116</v>
@@ -2234,33 +2234,33 @@
         <v>5.5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>2011</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <v>528</v>
@@ -2269,33 +2269,33 @@
         <v>8.6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>2024</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F7">
         <v>498</v>
@@ -2304,33 +2304,33 @@
         <v>8</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>1975</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>52</v>
@@ -2339,33 +2339,33 @@
         <v>4.2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>2008</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F9">
         <v>267</v>
@@ -2374,33 +2374,33 @@
         <v>7.8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>1925</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F10">
         <v>326</v>
@@ -2409,33 +2409,33 @@
         <v>6.9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D11">
         <v>2009</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F11">
         <v>437</v>
@@ -2444,33 +2444,33 @@
         <v>7.4</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D12">
         <v>2007</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F12">
         <v>948</v>
@@ -2479,33 +2479,33 @@
         <v>8.6</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D13">
         <v>1991</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F13">
         <v>383</v>
@@ -2514,33 +2514,33 @@
         <v>6.6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D14">
         <v>2024</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F14">
         <v>56</v>
@@ -2549,33 +2549,33 @@
         <v>4.3</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D15">
         <v>1989</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F15">
         <v>304</v>
@@ -2584,33 +2584,33 @@
         <v>5.3</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D16">
         <v>2017</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F16">
         <v>940</v>
@@ -2619,33 +2619,33 @@
         <v>9.1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D17">
         <v>2019</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F17">
         <v>376</v>
@@ -2654,33 +2654,33 @@
         <v>7.4</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D18">
         <v>2002</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F18">
         <v>221</v>
@@ -2689,33 +2689,33 @@
         <v>6.6</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
         <v>96</v>
-      </c>
-      <c r="J18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" t="s">
-        <v>99</v>
       </c>
       <c r="D19">
         <v>2011</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F19">
         <v>272</v>
@@ -2724,33 +2724,33 @@
         <v>6.3</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D20">
         <v>2011</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F20">
         <v>289</v>
@@ -2759,33 +2759,33 @@
         <v>6.6</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D21">
         <v>2011</v>
       </c>
       <c r="E21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F21">
         <v>311</v>
@@ -2794,33 +2794,33 @@
         <v>6.2</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D22">
         <v>2011</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F22">
         <v>321</v>
@@ -2829,33 +2829,33 @@
         <v>6.4</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D23">
         <v>2014</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F23">
         <v>112</v>
@@ -2864,33 +2864,33 @@
         <v>6.4</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D24">
         <v>2014</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F24">
         <v>267</v>
@@ -2899,33 +2899,33 @@
         <v>6.3</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D25">
         <v>2014</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F25">
         <v>392</v>
@@ -2934,33 +2934,33 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D26">
         <v>2014</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F26">
         <v>383</v>
@@ -2969,33 +2969,33 @@
         <v>7.3</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D27">
         <v>2018</v>
       </c>
       <c r="E27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F27">
         <v>482</v>
@@ -3004,33 +3004,33 @@
         <v>6.4</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D28">
         <v>2018</v>
       </c>
       <c r="E28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F28">
         <v>392</v>
@@ -3039,33 +3039,33 @@
         <v>7.3</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D29">
         <v>2018</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F29">
         <v>298</v>
@@ -3074,33 +3074,33 @@
         <v>6.4</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D30">
         <v>2018</v>
       </c>
       <c r="E30" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F30">
         <v>242</v>
@@ -3109,33 +3109,33 @@
         <v>6.2</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D31">
         <v>1925</v>
       </c>
       <c r="E31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F31">
         <v>382</v>
@@ -3144,33 +3144,33 @@
         <v>7.3</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C32" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D32">
         <v>1925</v>
       </c>
       <c r="E32" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F32">
         <v>251</v>
@@ -3179,33 +3179,33 @@
         <v>7.4</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J32" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D33">
         <v>2006</v>
       </c>
       <c r="E33" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F33">
         <v>382</v>
@@ -3214,33 +3214,33 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J33" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D34">
         <v>2006</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F34">
         <v>364</v>
@@ -3249,33 +3249,33 @@
         <v>7.3</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D35">
         <v>2021</v>
       </c>
       <c r="E35" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F35">
         <v>322</v>
@@ -3284,33 +3284,33 @@
         <v>8.4</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J35" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C36" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D36">
         <v>1896</v>
       </c>
       <c r="E36" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F36">
         <v>112</v>
@@ -3319,33 +3319,33 @@
         <v>6.8</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J36" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C37" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D37">
         <v>1896</v>
       </c>
       <c r="E37" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F37">
         <v>324</v>
@@ -3354,33 +3354,33 @@
         <v>6.4</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C38" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D38">
         <v>2011</v>
       </c>
       <c r="E38" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F38">
         <v>390</v>
@@ -3389,33 +3389,33 @@
         <v>7.3</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J38" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C39" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D39">
         <v>2021</v>
       </c>
       <c r="E39" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F39">
         <v>432</v>
@@ -3424,33 +3424,33 @@
         <v>7.4</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J39" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C40" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D40">
         <v>2018</v>
       </c>
       <c r="E40" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F40">
         <v>530</v>
@@ -3459,33 +3459,33 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J40" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" t="s">
         <v>167</v>
-      </c>
-      <c r="C41" t="s">
-        <v>170</v>
       </c>
       <c r="D41">
         <v>1997</v>
       </c>
       <c r="E41" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F41">
         <v>567</v>
@@ -3494,33 +3494,33 @@
         <v>8</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J41" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C42" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D42">
         <v>1991</v>
       </c>
       <c r="E42" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F42">
         <v>321</v>
@@ -3529,33 +3529,33 @@
         <v>6.5</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C43" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D43">
         <v>2001</v>
       </c>
       <c r="E43" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F43">
         <v>153</v>
@@ -3564,33 +3564,33 @@
         <v>6.3</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J43" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C44" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D44">
         <v>2001</v>
       </c>
       <c r="E44" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F44">
         <v>968</v>
@@ -3599,33 +3599,33 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J44" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C45" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D45">
         <v>1992</v>
       </c>
       <c r="E45" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F45">
         <v>723</v>
@@ -3634,33 +3634,33 @@
         <v>9.1</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J45" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D46">
         <v>2012</v>
       </c>
       <c r="E46" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F46">
         <v>528</v>
@@ -3669,33 +3669,33 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J46" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D47">
         <v>2011</v>
       </c>
       <c r="E47" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F47">
         <v>428</v>
@@ -3704,33 +3704,33 @@
         <v>7.9</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J47" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C48" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D48">
         <v>2009</v>
       </c>
       <c r="E48" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F48">
         <v>563</v>
@@ -3739,33 +3739,33 @@
         <v>8.1</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="J48" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D49">
         <v>2011</v>
       </c>
       <c r="E49" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F49">
         <v>980</v>
@@ -3774,33 +3774,33 @@
         <v>9.5</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J49" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C50" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D50">
         <v>2018</v>
       </c>
       <c r="E50" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F50">
         <v>582</v>
@@ -3809,33 +3809,33 @@
         <v>7.1</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J50" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C51" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D51">
         <v>2015</v>
       </c>
       <c r="E51" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F51">
         <v>970</v>
@@ -3844,33 +3844,33 @@
         <v>6.3</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J51" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C52" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D52">
         <v>2013</v>
       </c>
       <c r="E52" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F52">
         <v>934</v>
@@ -3879,33 +3879,33 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="J52" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C53" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D53">
         <v>2014</v>
       </c>
       <c r="E53" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F53">
         <v>564</v>
@@ -3914,33 +3914,33 @@
         <v>6.3</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J53" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C54" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D54">
         <v>1948</v>
       </c>
       <c r="E54" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F54">
         <v>438</v>
@@ -3949,33 +3949,33 @@
         <v>6.4</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="J54" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K54" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C55" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D55">
         <v>1996</v>
       </c>
       <c r="E55" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F55">
         <v>930</v>
@@ -3984,33 +3984,33 @@
         <v>7.8</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J55" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K55" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C56" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D56">
         <v>2000</v>
       </c>
       <c r="E56" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F56">
         <v>589</v>
@@ -4019,33 +4019,33 @@
         <v>7.1</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="J56" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K56" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C57" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D57">
         <v>2010</v>
       </c>
       <c r="E57" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F57">
         <v>472</v>
@@ -4054,33 +4054,33 @@
         <v>6.3</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J57" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K57" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C58" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D58">
         <v>2014</v>
       </c>
       <c r="E58" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F58">
         <v>632</v>
@@ -4089,33 +4089,33 @@
         <v>7.9</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="J58" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K58" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C59" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D59">
         <v>2011</v>
       </c>
       <c r="E59" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F59">
         <v>467</v>
@@ -4124,33 +4124,33 @@
         <v>6.3</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="J59" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K59" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C60" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D60">
         <v>2004</v>
       </c>
       <c r="E60" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F60">
         <v>742</v>
@@ -4159,33 +4159,33 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="J60" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K60" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C61" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D61">
         <v>2005</v>
       </c>
       <c r="E61" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F61">
         <v>320</v>
@@ -4194,33 +4194,33 @@
         <v>6.2</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="J61" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K61" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C62" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D62">
         <v>2001</v>
       </c>
       <c r="E62" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F62">
         <v>428</v>
@@ -4229,33 +4229,33 @@
         <v>6.5</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="J62" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K62" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D63">
         <v>2004</v>
       </c>
       <c r="E63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F63">
         <v>320</v>
@@ -4264,33 +4264,33 @@
         <v>6.1</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="J63" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K63" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C64" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D64">
         <v>1997</v>
       </c>
       <c r="E64" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F64">
         <v>438</v>
@@ -4299,33 +4299,33 @@
         <v>7.1</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="J64" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K64" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C65" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D65">
         <v>2014</v>
       </c>
       <c r="E65" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F65">
         <v>638</v>
@@ -4334,33 +4334,33 @@
         <v>7.9</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J65" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K65" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C66" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D66">
         <v>1997</v>
       </c>
       <c r="E66" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F66">
         <v>532</v>
@@ -4369,33 +4369,33 @@
         <v>7.5</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="J66" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K66" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C67" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D67">
         <v>1991</v>
       </c>
       <c r="E67" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F67">
         <v>492</v>
@@ -4404,33 +4404,33 @@
         <v>6.2</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="J67" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K67" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C68" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D68">
         <v>2005</v>
       </c>
       <c r="E68" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F68">
         <v>319</v>
@@ -4439,33 +4439,33 @@
         <v>7.2</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="J68" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K68" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C69" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D69">
         <v>2015</v>
       </c>
       <c r="E69" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F69">
         <v>550</v>
@@ -4474,33 +4474,33 @@
         <v>7.6</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="J69" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K69" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C70" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D70">
         <v>2001</v>
       </c>
       <c r="E70" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F70">
         <v>689</v>
@@ -4509,33 +4509,33 @@
         <v>7.4</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="J70" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K70" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C71" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D71">
         <v>2009</v>
       </c>
       <c r="E71" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F71">
         <v>812</v>
@@ -4544,33 +4544,33 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="J71" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K71" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C72" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D72">
         <v>2005</v>
       </c>
       <c r="E72" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F72">
         <v>799</v>
@@ -4579,33 +4579,33 @@
         <v>8.1</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="J72" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K72" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C73" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D73">
         <v>2004</v>
       </c>
       <c r="E73" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F73">
         <v>729</v>
@@ -4614,33 +4614,33 @@
         <v>7.9</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="J73" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K73" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C74" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D74">
         <v>2018</v>
       </c>
       <c r="E74" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F74">
         <v>1034</v>
@@ -4649,33 +4649,33 @@
         <v>8.1</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="J74" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K74" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C75" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D75">
         <v>2008</v>
       </c>
       <c r="E75" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F75">
         <v>732</v>
@@ -4684,33 +4684,33 @@
         <v>7.2</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J75" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K75" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C76" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D76">
         <v>2004</v>
       </c>
       <c r="E76" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F76">
         <v>812</v>
@@ -4719,31 +4719,31 @@
         <v>7.5</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I76" s="1"/>
       <c r="J76" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K76" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C77" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D77">
         <v>2001</v>
       </c>
       <c r="E77" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F77">
         <v>742</v>
@@ -4752,33 +4752,33 @@
         <v>6.1</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="J77" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K77" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C78" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D78">
         <v>2010</v>
       </c>
       <c r="E78" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F78">
         <v>342</v>
@@ -4787,33 +4787,33 @@
         <v>6.7</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="J78" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K78" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C79" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D79">
         <v>2014</v>
       </c>
       <c r="E79" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F79">
         <v>490</v>
@@ -4822,33 +4822,33 @@
         <v>7.1</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="J79" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K79" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C80" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D80">
         <v>2015</v>
       </c>
       <c r="E80" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F80">
         <v>1132</v>
@@ -4857,33 +4857,33 @@
         <v>8.5</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J80" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K80" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C81" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D81">
         <v>2015</v>
       </c>
       <c r="E81" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F81">
         <v>983</v>
@@ -4892,33 +4892,33 @@
         <v>8.1</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="J81" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K81" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C82" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D82">
         <v>2017</v>
       </c>
       <c r="E82" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F82">
         <v>821</v>
@@ -4927,33 +4927,33 @@
         <v>7.9</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J82" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K82" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C83" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D83">
         <v>2013</v>
       </c>
       <c r="E83" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F83">
         <v>723</v>
@@ -4962,33 +4962,33 @@
         <v>8.1</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="J83" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K83" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C84" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D84">
         <v>2010</v>
       </c>
       <c r="E84" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F84">
         <v>690</v>
@@ -4997,16 +4997,16 @@
         <v>6.3</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J84" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K84" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>